<commit_message>
master covid analysis and refactor for new responses
</commit_message>
<xml_diff>
--- a/survey analysis/veteran's survey data/veteran's survey complete n=565.xlsx
+++ b/survey analysis/veteran's survey data/veteran's survey complete n=565.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJR52\Desktop\Veteran's Survey Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJR52\Documents\c3rn_veteran\Survey Analysis\veteran's survey data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA98697-799B-4DFD-9C0B-84DC58C639DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152DCD13-C5E6-43D4-8C7E-7CDC78B0195E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3780" windowWidth="21600" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="2960" windowWidth="14460" windowHeight="14950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal Veterans Survey Draft " sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3724" uniqueCount="1490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3694" uniqueCount="1490">
   <si>
     <t>Fair</t>
   </si>
@@ -5508,30 +5508,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A914" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H1628" sqref="H1628"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="M638" sqref="M638"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" customHeight="1" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="23" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="31.6328125" style="9" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="11.36328125" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="5.54296875" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="7.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="6" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="10.08984375" style="17" customWidth="1"/>
-    <col min="10" max="10" width="4.6328125" style="23" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="31.36328125" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="12.453125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="10.7265625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.90625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="13.1796875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="32.1796875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="19" width="8.7265625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="8.7265625" collapsed="1"/>
+    <col min="1" max="1" width="4.7265625" style="23" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="31.6328125" style="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="11.36328125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.54296875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="9.453125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="5.54296875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="7.1796875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10.08984375" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="4.6328125" style="23" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="31.36328125" style="9" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="12.453125" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="10.7265625" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.90625" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="13.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="32.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="19" width="8.7265625" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -16618,9 +16617,6 @@
         <v>38</v>
       </c>
       <c r="D487" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E487" s="6" t="s">
         <v>1485</v>
       </c>
       <c r="F487" s="6"/>
@@ -16636,9 +16632,6 @@
         <v>39</v>
       </c>
       <c r="M487" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N487" s="6" t="s">
         <v>1485</v>
       </c>
     </row>
@@ -16650,9 +16643,6 @@
         <v>345</v>
       </c>
       <c r="D488" s="1">
-        <v>0.38250000000000001</v>
-      </c>
-      <c r="E488" s="1">
         <v>0.61060000000000003</v>
       </c>
       <c r="F488" s="1"/>
@@ -16665,9 +16655,6 @@
         <v>120</v>
       </c>
       <c r="M488" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="N488" s="1">
         <v>0.59699999999999998</v>
       </c>
     </row>
@@ -16679,9 +16666,6 @@
         <v>299</v>
       </c>
       <c r="D489" s="1">
-        <v>0.33150000000000002</v>
-      </c>
-      <c r="E489" s="1">
         <v>0.5292</v>
       </c>
       <c r="F489" s="1"/>
@@ -16694,9 +16678,6 @@
         <v>100</v>
       </c>
       <c r="M489" s="1">
-        <v>0.3125</v>
-      </c>
-      <c r="N489" s="1">
         <v>0.4975</v>
       </c>
     </row>
@@ -16708,9 +16689,6 @@
         <v>197</v>
       </c>
       <c r="D490" s="1">
-        <v>0.21840000000000001</v>
-      </c>
-      <c r="E490" s="1">
         <v>0.34870000000000001</v>
       </c>
       <c r="F490" s="1"/>
@@ -16723,9 +16701,6 @@
         <v>84</v>
       </c>
       <c r="M490" s="1">
-        <v>0.26250000000000001</v>
-      </c>
-      <c r="N490" s="1">
         <v>0.41789999999999999</v>
       </c>
     </row>
@@ -16737,9 +16712,6 @@
         <v>37</v>
       </c>
       <c r="D491" s="1">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="E491" s="1">
         <v>6.5500000000000003E-2</v>
       </c>
       <c r="F491" s="1"/>
@@ -16752,9 +16724,6 @@
         <v>12</v>
       </c>
       <c r="M491" s="1">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="N491" s="1">
         <v>5.9700000000000003E-2</v>
       </c>
     </row>
@@ -16766,9 +16735,6 @@
         <v>24</v>
       </c>
       <c r="D492" s="1">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="E492" s="1">
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="F492" s="1"/>
@@ -16781,9 +16747,6 @@
         <v>4</v>
       </c>
       <c r="M492" s="1">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="N492" s="1">
         <v>1.9900000000000001E-2</v>
       </c>
     </row>
@@ -18075,9 +18038,6 @@
         <v>38</v>
       </c>
       <c r="D547" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E547" s="6" t="s">
         <v>1485</v>
       </c>
       <c r="F547" s="6"/>
@@ -18093,9 +18053,6 @@
         <v>39</v>
       </c>
       <c r="M547" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N547" s="6" t="s">
         <v>1485</v>
       </c>
       <c r="U547" s="43"/>
@@ -18108,9 +18065,6 @@
         <v>320</v>
       </c>
       <c r="D548" s="1">
-        <v>0.15559999999999999</v>
-      </c>
-      <c r="E548" s="1">
         <v>0.56640000000000001</v>
       </c>
       <c r="F548" s="1"/>
@@ -18123,9 +18077,6 @@
         <v>102</v>
       </c>
       <c r="M548" s="1">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="N548" s="1">
         <v>0.50749999999999995</v>
       </c>
       <c r="U548" s="43"/>
@@ -18138,9 +18089,6 @@
         <v>315</v>
       </c>
       <c r="D549" s="1">
-        <v>0.1532</v>
-      </c>
-      <c r="E549" s="1">
         <v>0.5575</v>
       </c>
       <c r="F549" s="1"/>
@@ -18153,9 +18101,6 @@
         <v>101</v>
       </c>
       <c r="M549" s="1">
-        <v>0.16189999999999999</v>
-      </c>
-      <c r="N549" s="1">
         <v>0.50249999999999995</v>
       </c>
       <c r="U549" s="43"/>
@@ -18168,9 +18113,6 @@
         <v>293</v>
       </c>
       <c r="D550" s="1">
-        <v>0.14249999999999999</v>
-      </c>
-      <c r="E550" s="1">
         <v>0.51859999999999995</v>
       </c>
       <c r="F550" s="1"/>
@@ -18183,9 +18125,6 @@
         <v>91</v>
       </c>
       <c r="M550" s="1">
-        <v>0.14580000000000001</v>
-      </c>
-      <c r="N550" s="1">
         <v>0.45269999999999999</v>
       </c>
       <c r="U550" s="43"/>
@@ -18198,9 +18137,6 @@
         <v>270</v>
       </c>
       <c r="D551" s="1">
-        <v>0.1313</v>
-      </c>
-      <c r="E551" s="1">
         <v>0.47789999999999999</v>
       </c>
       <c r="F551" s="1"/>
@@ -18213,9 +18149,6 @@
         <v>83</v>
       </c>
       <c r="M551" s="1">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="N551" s="1">
         <v>0.41289999999999999</v>
       </c>
       <c r="U551" s="43"/>
@@ -18228,9 +18161,6 @@
         <v>149</v>
       </c>
       <c r="D552" s="1">
-        <v>7.2499999999999995E-2</v>
-      </c>
-      <c r="E552" s="1">
         <v>0.26369999999999999</v>
       </c>
       <c r="F552" s="1"/>
@@ -18243,9 +18173,6 @@
         <v>48</v>
       </c>
       <c r="M552" s="1">
-        <v>7.6899999999999996E-2</v>
-      </c>
-      <c r="N552" s="1">
         <v>0.23880000000000001</v>
       </c>
       <c r="U552" s="43"/>
@@ -18258,9 +18185,6 @@
         <v>122</v>
       </c>
       <c r="D553" s="1">
-        <v>5.9299999999999999E-2</v>
-      </c>
-      <c r="E553" s="1">
         <v>0.21590000000000001</v>
       </c>
       <c r="F553" s="1"/>
@@ -18273,9 +18197,6 @@
         <v>35</v>
       </c>
       <c r="M553" s="1">
-        <v>5.6099999999999997E-2</v>
-      </c>
-      <c r="N553" s="1">
         <v>0.1741</v>
       </c>
       <c r="U553" s="43"/>
@@ -18288,9 +18209,6 @@
         <v>115</v>
       </c>
       <c r="D554" s="1">
-        <v>5.5899999999999998E-2</v>
-      </c>
-      <c r="E554" s="1">
         <v>0.20349999999999999</v>
       </c>
       <c r="F554" s="1"/>
@@ -18303,9 +18221,6 @@
         <v>32</v>
       </c>
       <c r="M554" s="1">
-        <v>5.1299999999999998E-2</v>
-      </c>
-      <c r="N554" s="1">
         <v>0.15920000000000001</v>
       </c>
       <c r="U554" s="43"/>
@@ -18318,9 +18233,6 @@
         <v>111</v>
       </c>
       <c r="D555" s="1">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E555" s="1">
         <v>0.19650000000000001</v>
       </c>
       <c r="F555" s="1"/>
@@ -18333,9 +18245,6 @@
         <v>30</v>
       </c>
       <c r="M555" s="1">
-        <v>4.8099999999999997E-2</v>
-      </c>
-      <c r="N555" s="1">
         <v>0.14929999999999999</v>
       </c>
       <c r="U555" s="43"/>
@@ -18348,9 +18257,6 @@
         <v>94</v>
       </c>
       <c r="D556" s="1">
-        <v>4.5699999999999998E-2</v>
-      </c>
-      <c r="E556" s="1">
         <v>0.16639999999999999</v>
       </c>
       <c r="F556" s="1"/>
@@ -18363,9 +18269,6 @@
         <v>29</v>
       </c>
       <c r="M556" s="1">
-        <v>4.65E-2</v>
-      </c>
-      <c r="N556" s="1">
         <v>0.14430000000000001</v>
       </c>
       <c r="U556" s="43"/>
@@ -18378,9 +18281,6 @@
         <v>90</v>
       </c>
       <c r="D557" s="1">
-        <v>4.3799999999999999E-2</v>
-      </c>
-      <c r="E557" s="1">
         <v>0.1593</v>
       </c>
       <c r="F557" s="1"/>
@@ -18393,9 +18293,6 @@
         <v>26</v>
       </c>
       <c r="M557" s="1">
-        <v>4.1700000000000001E-2</v>
-      </c>
-      <c r="N557" s="1">
         <v>0.12939999999999999</v>
       </c>
       <c r="U557" s="43"/>
@@ -18408,9 +18305,6 @@
         <v>64</v>
       </c>
       <c r="D558" s="1">
-        <v>3.1099999999999999E-2</v>
-      </c>
-      <c r="E558" s="1">
         <v>0.1133</v>
       </c>
       <c r="F558" s="1"/>
@@ -18423,9 +18317,6 @@
         <v>15</v>
       </c>
       <c r="M558" s="1">
-        <v>2.4E-2</v>
-      </c>
-      <c r="N558" s="1">
         <v>7.46E-2</v>
       </c>
       <c r="U558" s="43"/>
@@ -18438,9 +18329,6 @@
         <v>33</v>
       </c>
       <c r="D559" s="1">
-        <v>1.61E-2</v>
-      </c>
-      <c r="E559" s="1">
         <v>5.8400000000000001E-2</v>
       </c>
       <c r="F559" s="1"/>
@@ -18453,9 +18341,6 @@
         <v>15</v>
       </c>
       <c r="M559" s="1">
-        <v>2.4E-2</v>
-      </c>
-      <c r="N559" s="1">
         <v>7.46E-2</v>
       </c>
       <c r="U559" s="43"/>
@@ -18468,9 +18353,6 @@
         <v>21</v>
       </c>
       <c r="D560" s="1">
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="E560" s="1">
         <v>3.7199999999999997E-2</v>
       </c>
       <c r="F560" s="1"/>
@@ -18483,9 +18365,6 @@
         <v>7</v>
       </c>
       <c r="M560" s="1">
-        <v>1.12E-2</v>
-      </c>
-      <c r="N560" s="1">
         <v>3.4799999999999998E-2</v>
       </c>
       <c r="U560" s="43"/>
@@ -18498,9 +18377,6 @@
         <v>18</v>
       </c>
       <c r="D561" s="1">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="E561" s="1">
         <v>3.1899999999999998E-2</v>
       </c>
       <c r="F561" s="1"/>
@@ -18513,9 +18389,6 @@
         <v>3</v>
       </c>
       <c r="M561" s="1">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="N561" s="1">
         <v>1.49E-2</v>
       </c>
       <c r="U561" s="43"/>
@@ -18528,9 +18401,6 @@
         <v>16</v>
       </c>
       <c r="D562" s="1">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="E562" s="1">
         <v>2.8299999999999999E-2</v>
       </c>
       <c r="F562" s="1"/>
@@ -18543,9 +18413,6 @@
         <v>2</v>
       </c>
       <c r="M562" s="1">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="N562" s="1">
         <v>0.01</v>
       </c>
       <c r="U562" s="43"/>
@@ -18558,9 +18425,6 @@
         <v>12</v>
       </c>
       <c r="D563" s="1">
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="E563" s="1">
         <v>2.12E-2</v>
       </c>
       <c r="F563" s="1"/>
@@ -18573,9 +18437,6 @@
         <v>2</v>
       </c>
       <c r="M563" s="1">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="N563" s="1">
         <v>0.01</v>
       </c>
       <c r="U563" s="43"/>
@@ -18588,9 +18449,6 @@
         <v>7</v>
       </c>
       <c r="D564" s="1">
-        <v>3.3999999999999998E-3</v>
-      </c>
-      <c r="E564" s="1">
         <v>1.24E-2</v>
       </c>
       <c r="F564" s="1"/>
@@ -18603,9 +18461,6 @@
         <v>2</v>
       </c>
       <c r="M564" s="1">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="N564" s="1">
         <v>0.01</v>
       </c>
       <c r="U564" s="43"/>
@@ -18618,9 +18473,6 @@
         <v>6</v>
       </c>
       <c r="D565" s="1">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E565" s="1">
         <v>1.06E-2</v>
       </c>
       <c r="F565" s="1"/>
@@ -18633,17 +18485,11 @@
         <v>1</v>
       </c>
       <c r="M565" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N565" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="566" spans="1:21" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="C566" s="7">
-        <f>SUM(C548:C565)</f>
-        <v>2056</v>
-      </c>
+      <c r="C566" s="7"/>
       <c r="L566" s="7">
         <f>SUM(L548:L565)</f>
         <v>624</v>
@@ -20373,9 +20219,6 @@
         <v>38</v>
       </c>
       <c r="D629" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E629" s="6" t="s">
         <v>1485</v>
       </c>
       <c r="F629" s="6"/>
@@ -20391,9 +20234,6 @@
         <v>39</v>
       </c>
       <c r="M629" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N629" s="6" t="s">
         <v>1485</v>
       </c>
     </row>
@@ -20405,9 +20245,6 @@
         <v>168</v>
       </c>
       <c r="D630" s="1">
-        <v>0.1298</v>
-      </c>
-      <c r="E630" s="1">
         <v>0.29730000000000001</v>
       </c>
       <c r="F630" s="1"/>
@@ -20420,9 +20257,6 @@
         <v>65</v>
       </c>
       <c r="M630" s="1">
-        <v>0.13919999999999999</v>
-      </c>
-      <c r="N630" s="1">
         <v>0.32340000000000002</v>
       </c>
       <c r="U630" s="42"/>
@@ -20436,9 +20270,6 @@
         <v>147</v>
       </c>
       <c r="D631" s="1">
-        <v>0.11360000000000001</v>
-      </c>
-      <c r="E631" s="1">
         <v>0.26019999999999999</v>
       </c>
       <c r="F631" s="1"/>
@@ -20451,9 +20282,6 @@
         <v>53</v>
       </c>
       <c r="M631" s="1">
-        <v>0.1135</v>
-      </c>
-      <c r="N631" s="1">
         <v>0.26369999999999999</v>
       </c>
     </row>
@@ -20465,9 +20293,6 @@
         <v>133</v>
       </c>
       <c r="D632" s="1">
-        <v>0.1028</v>
-      </c>
-      <c r="E632" s="1">
         <v>0.2354</v>
       </c>
       <c r="F632" s="1"/>
@@ -20480,9 +20305,6 @@
         <v>39</v>
       </c>
       <c r="M632" s="1">
-        <v>8.3500000000000005E-2</v>
-      </c>
-      <c r="N632" s="1">
         <v>0.19400000000000001</v>
       </c>
       <c r="U632" s="42"/>
@@ -20496,9 +20318,6 @@
         <v>103</v>
       </c>
       <c r="D633" s="1">
-        <v>7.9600000000000004E-2</v>
-      </c>
-      <c r="E633" s="1">
         <v>0.18229999999999999</v>
       </c>
       <c r="F633" s="1"/>
@@ -20511,9 +20330,6 @@
         <v>39</v>
       </c>
       <c r="M633" s="1">
-        <v>8.3500000000000005E-2</v>
-      </c>
-      <c r="N633" s="1">
         <v>0.19400000000000001</v>
       </c>
       <c r="U633" s="31"/>
@@ -20527,9 +20343,6 @@
         <v>98</v>
       </c>
       <c r="D634" s="1">
-        <v>7.5700000000000003E-2</v>
-      </c>
-      <c r="E634" s="1">
         <v>0.17349999999999999</v>
       </c>
       <c r="F634" s="1"/>
@@ -20542,17 +20355,10 @@
         <v>39</v>
       </c>
       <c r="M634" s="1">
-        <v>8.3500000000000005E-2</v>
-      </c>
-      <c r="N634" s="1">
         <v>0.19400000000000001</v>
       </c>
-      <c r="U634" s="42" t="s">
-        <v>182</v>
-      </c>
-      <c r="V634" s="43">
-        <v>0.26019999999999999</v>
-      </c>
+      <c r="U634" s="42"/>
+      <c r="V634" s="43"/>
     </row>
     <row r="635" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B635" s="31" t="s">
@@ -20562,9 +20368,6 @@
         <v>94</v>
       </c>
       <c r="D635" s="1">
-        <v>7.2599999999999998E-2</v>
-      </c>
-      <c r="E635" s="1">
         <v>0.16639999999999999</v>
       </c>
       <c r="F635" s="1"/>
@@ -20577,17 +20380,10 @@
         <v>36</v>
       </c>
       <c r="M635" s="1">
-        <v>7.7100000000000002E-2</v>
-      </c>
-      <c r="N635" s="1">
         <v>0.17910000000000001</v>
       </c>
-      <c r="U635" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="V635" s="43">
-        <v>0.17349999999999999</v>
-      </c>
+      <c r="U635" s="42"/>
+      <c r="V635" s="43"/>
     </row>
     <row r="636" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B636" s="31" t="s">
@@ -20597,9 +20393,6 @@
         <v>88</v>
       </c>
       <c r="D636" s="1">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="E636" s="1">
         <v>0.15579999999999999</v>
       </c>
       <c r="F636" s="1"/>
@@ -20612,17 +20405,10 @@
         <v>32</v>
       </c>
       <c r="M636" s="1">
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="N636" s="1">
         <v>0.15920000000000001</v>
       </c>
-      <c r="U636" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="V636" s="43">
-        <v>0.16639999999999999</v>
-      </c>
+      <c r="U636" s="31"/>
+      <c r="V636" s="43"/>
     </row>
     <row r="637" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B637" s="32" t="s">
@@ -20632,9 +20418,6 @@
         <v>79</v>
       </c>
       <c r="D637" s="1">
-        <v>6.1100000000000002E-2</v>
-      </c>
-      <c r="E637" s="1">
         <v>0.13980000000000001</v>
       </c>
       <c r="F637" s="1"/>
@@ -20647,17 +20430,10 @@
         <v>32</v>
       </c>
       <c r="M637" s="1">
-        <v>6.8500000000000005E-2</v>
-      </c>
-      <c r="N637" s="1">
         <v>0.15920000000000001</v>
       </c>
-      <c r="U637" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="V637" s="43">
-        <v>0.15579999999999999</v>
-      </c>
+      <c r="U637" s="31"/>
+      <c r="V637" s="43"/>
     </row>
     <row r="638" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B638" s="32" t="s">
@@ -20667,9 +20443,6 @@
         <v>74</v>
       </c>
       <c r="D638" s="1">
-        <v>5.7200000000000001E-2</v>
-      </c>
-      <c r="E638" s="1">
         <v>0.13100000000000001</v>
       </c>
       <c r="F638" s="1"/>
@@ -20682,17 +20455,10 @@
         <v>27</v>
       </c>
       <c r="M638" s="1">
-        <v>5.7799999999999997E-2</v>
-      </c>
-      <c r="N638" s="1">
         <v>0.1343</v>
       </c>
-      <c r="U638" s="42" t="s">
-        <v>188</v>
-      </c>
-      <c r="V638" s="43">
-        <v>0.13980000000000001</v>
-      </c>
+      <c r="U638" s="42"/>
+      <c r="V638" s="43"/>
     </row>
     <row r="639" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B639" s="32" t="s">
@@ -20702,9 +20468,6 @@
         <v>63</v>
       </c>
       <c r="D639" s="1">
-        <v>4.87E-2</v>
-      </c>
-      <c r="E639" s="1">
         <v>0.1115</v>
       </c>
       <c r="F639" s="1"/>
@@ -20717,17 +20480,10 @@
         <v>27</v>
       </c>
       <c r="M639" s="1">
-        <v>5.7799999999999997E-2</v>
-      </c>
-      <c r="N639" s="1">
         <v>0.1343</v>
       </c>
-      <c r="U639" s="42" t="s">
-        <v>187</v>
-      </c>
-      <c r="V639" s="43">
-        <v>0.1115</v>
-      </c>
+      <c r="U639" s="42"/>
+      <c r="V639" s="43"/>
     </row>
     <row r="640" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B640" s="31" t="s">
@@ -20737,9 +20493,6 @@
         <v>39</v>
       </c>
       <c r="D640" s="1">
-        <v>3.0099999999999998E-2</v>
-      </c>
-      <c r="E640" s="1">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="F640" s="1"/>
@@ -20752,17 +20505,10 @@
         <v>11</v>
       </c>
       <c r="M640" s="1">
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="N640" s="1">
         <v>5.4699999999999999E-2</v>
       </c>
-      <c r="U640" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="V640" s="43">
-        <v>6.9000000000000006E-2</v>
-      </c>
+      <c r="U640" s="31"/>
+      <c r="V640" s="43"/>
     </row>
     <row r="641" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B641" s="31" t="s">
@@ -20772,9 +20518,6 @@
         <v>29</v>
       </c>
       <c r="D641" s="1">
-        <v>2.24E-2</v>
-      </c>
-      <c r="E641" s="1">
         <v>5.1299999999999998E-2</v>
       </c>
       <c r="F641" s="1"/>
@@ -20787,17 +20530,10 @@
         <v>10</v>
       </c>
       <c r="M641" s="1">
-        <v>2.1399999999999999E-2</v>
-      </c>
-      <c r="N641" s="1">
         <v>4.9799999999999997E-2</v>
       </c>
-      <c r="U641" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="V641" s="43">
-        <v>5.1299999999999998E-2</v>
-      </c>
+      <c r="U641" s="31"/>
+      <c r="V641" s="43"/>
     </row>
     <row r="642" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B642" s="31" t="s">
@@ -20807,9 +20543,6 @@
         <v>25</v>
       </c>
       <c r="D642" s="1">
-        <v>1.9300000000000001E-2</v>
-      </c>
-      <c r="E642" s="1">
         <v>4.4200000000000003E-2</v>
       </c>
       <c r="F642" s="1"/>
@@ -20822,17 +20555,10 @@
         <v>7</v>
       </c>
       <c r="M642" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N642" s="1">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="U642" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="V642" s="43">
-        <v>4.4200000000000003E-2</v>
-      </c>
+      <c r="U642" s="31"/>
+      <c r="V642" s="43"/>
     </row>
     <row r="643" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B643" s="32" t="s">
@@ -20842,9 +20568,6 @@
         <v>24</v>
       </c>
       <c r="D643" s="1">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="E643" s="1">
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="F643" s="1"/>
@@ -20857,17 +20580,10 @@
         <v>7</v>
       </c>
       <c r="M643" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N643" s="1">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="U643" s="42" t="s">
-        <v>195</v>
-      </c>
-      <c r="V643" s="43">
-        <v>4.2500000000000003E-2</v>
-      </c>
+      <c r="U643" s="42"/>
+      <c r="V643" s="43"/>
     </row>
     <row r="644" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B644" s="31" t="s">
@@ -20877,9 +20593,6 @@
         <v>22</v>
       </c>
       <c r="D644" s="1">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="E644" s="1">
         <v>3.8899999999999997E-2</v>
       </c>
       <c r="F644" s="1"/>
@@ -20892,17 +20605,10 @@
         <v>7</v>
       </c>
       <c r="M644" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N644" s="1">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="U644" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="V644" s="43">
-        <v>3.8899999999999997E-2</v>
-      </c>
+      <c r="U644" s="31"/>
+      <c r="V644" s="43"/>
     </row>
     <row r="645" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B645" s="31" t="s">
@@ -20912,9 +20618,6 @@
         <v>21</v>
       </c>
       <c r="D645" s="1">
-        <v>1.6199999999999999E-2</v>
-      </c>
-      <c r="E645" s="1">
         <v>3.7199999999999997E-2</v>
       </c>
       <c r="F645" s="1"/>
@@ -20927,17 +20630,10 @@
         <v>7</v>
       </c>
       <c r="M645" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N645" s="1">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="U645" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="V645" s="43">
-        <v>3.7199999999999997E-2</v>
-      </c>
+      <c r="U645" s="31"/>
+      <c r="V645" s="43"/>
     </row>
     <row r="646" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B646" s="31" t="s">
@@ -20947,9 +20643,6 @@
         <v>19</v>
       </c>
       <c r="D646" s="1">
-        <v>1.47E-2</v>
-      </c>
-      <c r="E646" s="1">
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="F646" s="1"/>
@@ -20962,17 +20655,10 @@
         <v>7</v>
       </c>
       <c r="M646" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N646" s="1">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="U646" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="V646" s="43">
-        <v>3.3599999999999998E-2</v>
-      </c>
+      <c r="U646" s="31"/>
+      <c r="V646" s="43"/>
     </row>
     <row r="647" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B647" s="31" t="s">
@@ -20982,9 +20668,6 @@
         <v>18</v>
       </c>
       <c r="D647" s="1">
-        <v>1.3899999999999999E-2</v>
-      </c>
-      <c r="E647" s="1">
         <v>3.1899999999999998E-2</v>
       </c>
       <c r="F647" s="1"/>
@@ -20997,17 +20680,10 @@
         <v>6</v>
       </c>
       <c r="M647" s="1">
-        <v>1.2800000000000001E-2</v>
-      </c>
-      <c r="N647" s="1">
         <v>2.9899999999999999E-2</v>
       </c>
-      <c r="U647" s="31" t="s">
-        <v>190</v>
-      </c>
-      <c r="V647" s="43">
-        <v>3.1899999999999998E-2</v>
-      </c>
+      <c r="U647" s="31"/>
+      <c r="V647" s="43"/>
     </row>
     <row r="648" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B648" s="31" t="s">
@@ -21017,9 +20693,6 @@
         <v>15</v>
       </c>
       <c r="D648" s="1">
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="E648" s="1">
         <v>2.6499999999999999E-2</v>
       </c>
       <c r="F648" s="1"/>
@@ -21032,17 +20705,10 @@
         <v>5</v>
       </c>
       <c r="M648" s="1">
-        <v>1.0699999999999999E-2</v>
-      </c>
-      <c r="N648" s="1">
         <v>2.4899999999999999E-2</v>
       </c>
-      <c r="U648" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="V648" s="43">
-        <v>2.6499999999999999E-2</v>
-      </c>
+      <c r="U648" s="31"/>
+      <c r="V648" s="43"/>
     </row>
     <row r="649" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B649" s="31" t="s">
@@ -21052,9 +20718,6 @@
         <v>10</v>
       </c>
       <c r="D649" s="1">
-        <v>7.7000000000000002E-3</v>
-      </c>
-      <c r="E649" s="1">
         <v>1.77E-2</v>
       </c>
       <c r="F649" s="1"/>
@@ -21067,17 +20730,10 @@
         <v>5</v>
       </c>
       <c r="M649" s="1">
-        <v>1.0699999999999999E-2</v>
-      </c>
-      <c r="N649" s="1">
         <v>2.4899999999999999E-2</v>
       </c>
-      <c r="U649" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="V649" s="43">
-        <v>1.77E-2</v>
-      </c>
+      <c r="U649" s="31"/>
+      <c r="V649" s="43"/>
     </row>
     <row r="650" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B650" s="31" t="s">
@@ -21087,9 +20743,6 @@
         <v>9</v>
       </c>
       <c r="D650" s="1">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E650" s="1">
         <v>1.5900000000000001E-2</v>
       </c>
       <c r="F650" s="1"/>
@@ -21102,17 +20755,10 @@
         <v>4</v>
       </c>
       <c r="M650" s="1">
-        <v>8.6E-3</v>
-      </c>
-      <c r="N650" s="1">
         <v>1.9900000000000001E-2</v>
       </c>
-      <c r="U650" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="V650" s="43">
-        <v>1.5900000000000001E-2</v>
-      </c>
+      <c r="U650" s="31"/>
+      <c r="V650" s="43"/>
     </row>
     <row r="651" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B651" s="31" t="s">
@@ -21122,9 +20768,6 @@
         <v>8</v>
       </c>
       <c r="D651" s="1">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="E651" s="1">
         <v>1.4200000000000001E-2</v>
       </c>
       <c r="F651" s="1"/>
@@ -21137,17 +20780,10 @@
         <v>1</v>
       </c>
       <c r="M651" s="1">
-        <v>2.0999999999999999E-3</v>
-      </c>
-      <c r="N651" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="U651" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="V651" s="43">
-        <v>1.4200000000000001E-2</v>
-      </c>
+      <c r="U651" s="31"/>
+      <c r="V651" s="43"/>
     </row>
     <row r="652" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B652" s="31" t="s">
@@ -21157,9 +20793,6 @@
         <v>5</v>
       </c>
       <c r="D652" s="1">
-        <v>3.8999999999999998E-3</v>
-      </c>
-      <c r="E652" s="1">
         <v>8.8000000000000005E-3</v>
       </c>
       <c r="F652" s="1"/>
@@ -21172,17 +20805,10 @@
         <v>1</v>
       </c>
       <c r="M652" s="1">
-        <v>2.0999999999999999E-3</v>
-      </c>
-      <c r="N652" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="U652" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="V652" s="43">
-        <v>8.8000000000000005E-3</v>
-      </c>
+      <c r="U652" s="31"/>
+      <c r="V652" s="43"/>
     </row>
     <row r="653" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B653" s="31" t="s">
@@ -21192,9 +20818,6 @@
         <v>3</v>
       </c>
       <c r="D653" s="1">
-        <v>2.3E-3</v>
-      </c>
-      <c r="E653" s="1">
         <v>5.3E-3</v>
       </c>
       <c r="F653" s="1"/>
@@ -21204,18 +20827,11 @@
         <f>SUM(L630:L652)</f>
         <v>467</v>
       </c>
-      <c r="U653" s="31" t="s">
-        <v>199</v>
-      </c>
-      <c r="V653" s="43">
-        <v>5.3E-3</v>
-      </c>
+      <c r="U653" s="31"/>
+      <c r="V653" s="43"/>
     </row>
     <row r="654" spans="1:22" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="C654" s="7">
-        <f>SUM(C630:C653)</f>
-        <v>1294</v>
-      </c>
+      <c r="C654" s="7"/>
     </row>
     <row r="655" spans="1:22" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A655" s="23" t="s">
@@ -22714,13 +22330,13 @@
         <v>0.32040000000000002</v>
       </c>
     </row>
-    <row r="737" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="737" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="C737" s="7">
         <f>SUM(C657:C736)</f>
         <v>565</v>
       </c>
     </row>
-    <row r="738" spans="1:14" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="738" spans="1:13" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A738" s="23" t="s">
         <v>327</v>
       </c>
@@ -22734,7 +22350,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="739" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="739" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A739" s="26" t="s">
         <v>42</v>
       </c>
@@ -22745,9 +22361,6 @@
         <v>38</v>
       </c>
       <c r="D739" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E739" s="6" t="s">
         <v>1485</v>
       </c>
       <c r="F739" s="6"/>
@@ -22763,13 +22376,10 @@
         <v>39</v>
       </c>
       <c r="M739" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N739" s="6" t="s">
         <v>1485</v>
       </c>
     </row>
-    <row r="740" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="740" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B740" s="31" t="s">
         <v>329</v>
       </c>
@@ -22777,9 +22387,6 @@
         <v>383</v>
       </c>
       <c r="D740" s="1">
-        <v>0.20710000000000001</v>
-      </c>
-      <c r="E740" s="1">
         <v>0.67789999999999995</v>
       </c>
       <c r="F740" s="1"/>
@@ -22792,13 +22399,10 @@
         <v>135</v>
       </c>
       <c r="M740" s="1">
-        <v>0.2228</v>
-      </c>
-      <c r="N740" s="1">
         <v>0.67159999999999997</v>
       </c>
     </row>
-    <row r="741" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="741" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B741" s="32" t="s">
         <v>330</v>
       </c>
@@ -22806,9 +22410,6 @@
         <v>335</v>
       </c>
       <c r="D741" s="1">
-        <v>0.1812</v>
-      </c>
-      <c r="E741" s="1">
         <v>0.59289999999999998</v>
       </c>
       <c r="F741" s="1"/>
@@ -22821,13 +22422,10 @@
         <v>113</v>
       </c>
       <c r="M741" s="1">
-        <v>0.1865</v>
-      </c>
-      <c r="N741" s="1">
         <v>0.56220000000000003</v>
       </c>
     </row>
-    <row r="742" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="742" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B742" s="31" t="s">
         <v>331</v>
       </c>
@@ -22835,9 +22433,6 @@
         <v>274</v>
       </c>
       <c r="D742" s="1">
-        <v>0.1482</v>
-      </c>
-      <c r="E742" s="1">
         <v>0.48499999999999999</v>
       </c>
       <c r="F742" s="1"/>
@@ -22850,13 +22445,10 @@
         <v>102</v>
       </c>
       <c r="M742" s="1">
-        <v>0.16830000000000001</v>
-      </c>
-      <c r="N742" s="1">
         <v>0.50749999999999995</v>
       </c>
     </row>
-    <row r="743" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="743" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B743" s="32" t="s">
         <v>333</v>
       </c>
@@ -22864,9 +22456,6 @@
         <v>199</v>
       </c>
       <c r="D743" s="1">
-        <v>0.1076</v>
-      </c>
-      <c r="E743" s="1">
         <v>0.35220000000000001</v>
       </c>
       <c r="F743" s="1"/>
@@ -22879,13 +22468,10 @@
         <v>60</v>
       </c>
       <c r="M743" s="1">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="N743" s="1">
         <v>0.29849999999999999</v>
       </c>
     </row>
-    <row r="744" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="744" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B744" s="31" t="s">
         <v>332</v>
       </c>
@@ -22893,9 +22479,6 @@
         <v>195</v>
       </c>
       <c r="D744" s="1">
-        <v>0.1055</v>
-      </c>
-      <c r="E744" s="1">
         <v>0.34510000000000002</v>
       </c>
       <c r="F744" s="1"/>
@@ -22908,13 +22491,10 @@
         <v>54</v>
       </c>
       <c r="M744" s="1">
-        <v>8.9099999999999999E-2</v>
-      </c>
-      <c r="N744" s="1">
         <v>0.26869999999999999</v>
       </c>
     </row>
-    <row r="745" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="745" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B745" s="31" t="s">
         <v>334</v>
       </c>
@@ -22922,9 +22502,6 @@
         <v>160</v>
       </c>
       <c r="D745" s="1">
-        <v>8.6499999999999994E-2</v>
-      </c>
-      <c r="E745" s="1">
         <v>0.28320000000000001</v>
       </c>
       <c r="F745" s="1"/>
@@ -22937,13 +22514,10 @@
         <v>53</v>
       </c>
       <c r="M745" s="1">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="N745" s="1">
         <v>0.26369999999999999</v>
       </c>
     </row>
-    <row r="746" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="746" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B746" s="31" t="s">
         <v>335</v>
       </c>
@@ -22951,9 +22525,6 @@
         <v>134</v>
       </c>
       <c r="D746" s="1">
-        <v>7.2499999999999995E-2</v>
-      </c>
-      <c r="E746" s="1">
         <v>0.23719999999999999</v>
       </c>
       <c r="F746" s="1"/>
@@ -22966,13 +22537,10 @@
         <v>41</v>
       </c>
       <c r="M746" s="1">
-        <v>6.7699999999999996E-2</v>
-      </c>
-      <c r="N746" s="1">
         <v>0.20399999999999999</v>
       </c>
     </row>
-    <row r="747" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="747" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B747" s="31" t="s">
         <v>336</v>
       </c>
@@ -22980,9 +22548,6 @@
         <v>84</v>
       </c>
       <c r="D747" s="1">
-        <v>4.5400000000000003E-2</v>
-      </c>
-      <c r="E747" s="1">
         <v>0.1487</v>
       </c>
       <c r="F747" s="1"/>
@@ -22995,13 +22560,10 @@
         <v>29</v>
       </c>
       <c r="M747" s="1">
-        <v>4.7899999999999998E-2</v>
-      </c>
-      <c r="N747" s="1">
         <v>0.14430000000000001</v>
       </c>
     </row>
-    <row r="748" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="748" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B748" s="31" t="s">
         <v>337</v>
       </c>
@@ -23009,9 +22571,6 @@
         <v>41</v>
       </c>
       <c r="D748" s="1">
-        <v>2.2200000000000001E-2</v>
-      </c>
-      <c r="E748" s="1">
         <v>7.2599999999999998E-2</v>
       </c>
       <c r="F748" s="1"/>
@@ -23024,13 +22583,10 @@
         <v>8</v>
       </c>
       <c r="M748" s="1">
-        <v>1.32E-2</v>
-      </c>
-      <c r="N748" s="1">
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="749" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="749" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B749" s="31" t="s">
         <v>24</v>
       </c>
@@ -23038,9 +22594,6 @@
         <v>22</v>
       </c>
       <c r="D749" s="1">
-        <v>1.1900000000000001E-2</v>
-      </c>
-      <c r="E749" s="1">
         <v>3.8899999999999997E-2</v>
       </c>
       <c r="F749" s="1"/>
@@ -23053,13 +22606,10 @@
         <v>8</v>
       </c>
       <c r="M749" s="1">
-        <v>1.32E-2</v>
-      </c>
-      <c r="N749" s="1">
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="750" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="750" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B750" s="31" t="s">
         <v>338</v>
       </c>
@@ -23067,9 +22617,6 @@
         <v>22</v>
       </c>
       <c r="D750" s="1">
-        <v>1.1900000000000001E-2</v>
-      </c>
-      <c r="E750" s="1">
         <v>3.8899999999999997E-2</v>
       </c>
       <c r="F750" s="1"/>
@@ -23082,23 +22629,17 @@
         <v>3</v>
       </c>
       <c r="M750" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N750" s="1">
         <v>1.49E-2</v>
       </c>
     </row>
-    <row r="751" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="C751" s="7">
-        <f>SUM(C740:C750)</f>
-        <v>1849</v>
-      </c>
+    <row r="751" spans="1:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="C751" s="7"/>
       <c r="L751" s="7">
         <f>SUM(L740:L750)</f>
         <v>606</v>
       </c>
     </row>
-    <row r="752" spans="1:14" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="752" spans="1:13" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A752" s="23" t="s">
         <v>339</v>
       </c>
@@ -25161,7 +24702,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="854" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="854" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A854" s="26" t="s">
         <v>42</v>
       </c>
@@ -25196,7 +24737,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="855" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="855" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B855" s="29">
         <v>100</v>
       </c>
@@ -25222,7 +24763,7 @@
         <v>72.378109449999997</v>
       </c>
     </row>
-    <row r="856" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="856" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B856" s="29">
         <v>0</v>
       </c>
@@ -25242,7 +24783,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="857" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="857" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B857" s="29">
         <v>50</v>
       </c>
@@ -25262,7 +24803,7 @@
         <v>2.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="858" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="858" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B858" s="29">
         <v>75</v>
       </c>
@@ -25282,7 +24823,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="859" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="859" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B859" s="29">
         <v>99</v>
       </c>
@@ -25302,7 +24843,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="860" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="860" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B860" s="29">
         <v>98</v>
       </c>
@@ -25322,7 +24863,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="861" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="861" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B861" s="29">
         <v>90</v>
       </c>
@@ -25342,7 +24883,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="862" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="862" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B862" s="29">
         <v>10</v>
       </c>
@@ -25362,7 +24903,7 @@
         <v>1.49E-2</v>
       </c>
     </row>
-    <row r="863" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="863" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B863" s="29">
         <v>1</v>
       </c>
@@ -25382,7 +24923,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="864" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="864" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B864" s="29">
         <v>97</v>
       </c>
@@ -25402,7 +24943,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="865" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="865" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B865" s="29">
         <v>30</v>
       </c>
@@ -25422,7 +24963,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="866" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="866" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B866" s="29">
         <v>80</v>
       </c>
@@ -25442,7 +24983,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="867" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="867" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B867" s="29">
         <v>25</v>
       </c>
@@ -25462,7 +25003,7 @@
         <v>2.9899999999999999E-2</v>
       </c>
     </row>
-    <row r="868" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="868" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B868" s="29">
         <v>5</v>
       </c>
@@ -25482,7 +25023,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="869" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="869" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B869" s="29">
         <v>96</v>
       </c>
@@ -25502,7 +25043,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="870" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="870" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B870" s="29">
         <v>95</v>
       </c>
@@ -25522,7 +25063,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="871" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="871" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B871" s="29">
         <v>15</v>
       </c>
@@ -25542,7 +25083,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="872" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="872" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B872" s="29">
         <v>4</v>
       </c>
@@ -25562,7 +25103,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="873" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="873" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B873" s="29">
         <v>2</v>
       </c>
@@ -25582,7 +25123,7 @@
         <v>4.48E-2</v>
       </c>
     </row>
-    <row r="874" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="874" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B874" s="29">
         <v>85</v>
       </c>
@@ -25602,7 +25143,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="875" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="875" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B875" s="29">
         <v>52</v>
       </c>
@@ -25622,7 +25163,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="876" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="876" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B876" s="29">
         <v>14</v>
       </c>
@@ -25642,7 +25183,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="877" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="877" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B877" s="29">
         <v>12</v>
       </c>
@@ -25662,7 +25203,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="878" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="878" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B878" s="29">
         <v>3</v>
       </c>
@@ -25682,7 +25223,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="879" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="879" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B879" s="29">
         <v>89</v>
       </c>
@@ -25702,7 +25243,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="880" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="880" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B880" s="29">
         <v>82</v>
       </c>
@@ -25722,7 +25263,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="881" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="881" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B881" s="29">
         <v>65</v>
       </c>
@@ -25742,7 +25283,7 @@
         <v>1.9900000000000001E-2</v>
       </c>
     </row>
-    <row r="882" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="882" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B882" s="29">
         <v>51</v>
       </c>
@@ -25762,7 +25303,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="883" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="883" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B883" s="29">
         <v>26</v>
       </c>
@@ -25782,7 +25323,7 @@
         <v>2.9899999999999999E-2</v>
       </c>
     </row>
-    <row r="884" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="884" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B884" s="29">
         <v>19</v>
       </c>
@@ -25802,7 +25343,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="885" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="885" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B885" s="29">
         <v>18</v>
       </c>
@@ -25822,7 +25363,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="886" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="886" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B886" s="29">
         <v>17</v>
       </c>
@@ -25842,7 +25383,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="887" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="887" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B887" s="29">
         <v>13</v>
       </c>
@@ -25862,7 +25403,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="888" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="888" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B888" s="29">
         <v>9</v>
       </c>
@@ -25882,7 +25423,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="889" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="889" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B889" s="29">
         <v>7</v>
       </c>
@@ -25902,7 +25443,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="890" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="890" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B890" s="29">
         <v>6</v>
       </c>
@@ -25922,7 +25463,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="891" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="891" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B891" s="29">
         <v>94</v>
       </c>
@@ -25942,7 +25483,7 @@
         <v>1.9900000000000001E-2</v>
       </c>
     </row>
-    <row r="892" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="892" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B892" s="29">
         <v>93</v>
       </c>
@@ -25962,7 +25503,7 @@
         <v>8.4599999999999995E-2</v>
       </c>
     </row>
-    <row r="893" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="893" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B893" s="29">
         <v>91</v>
       </c>
@@ -25978,7 +25519,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="894" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="894" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B894" s="29">
         <v>87</v>
       </c>
@@ -25990,7 +25531,7 @@
       </c>
       <c r="K894"/>
     </row>
-    <row r="895" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="895" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B895" s="29">
         <v>86</v>
       </c>
@@ -26002,7 +25543,7 @@
       </c>
       <c r="K895"/>
     </row>
-    <row r="896" spans="2:13" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="896" spans="2:13" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B896" s="29">
         <v>84</v>
       </c>
@@ -26014,7 +25555,7 @@
       </c>
       <c r="K896"/>
     </row>
-    <row r="897" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="897" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B897" s="29">
         <v>81</v>
       </c>
@@ -26026,7 +25567,7 @@
       </c>
       <c r="K897"/>
     </row>
-    <row r="898" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="898" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B898" s="29">
         <v>73</v>
       </c>
@@ -26038,7 +25579,7 @@
       </c>
       <c r="K898"/>
     </row>
-    <row r="899" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="899" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B899" s="29">
         <v>70</v>
       </c>
@@ -26050,7 +25591,7 @@
       </c>
       <c r="K899"/>
     </row>
-    <row r="900" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="900" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B900" s="29">
         <v>67</v>
       </c>
@@ -26062,7 +25603,7 @@
       </c>
       <c r="K900"/>
     </row>
-    <row r="901" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="901" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B901" s="29">
         <v>61</v>
       </c>
@@ -26074,7 +25615,7 @@
       </c>
       <c r="K901"/>
     </row>
-    <row r="902" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="902" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B902" s="29">
         <v>56</v>
       </c>
@@ -26086,7 +25627,7 @@
       </c>
       <c r="K902"/>
     </row>
-    <row r="903" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="903" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B903" s="29">
         <v>49</v>
       </c>
@@ -26098,7 +25639,7 @@
       </c>
       <c r="K903"/>
     </row>
-    <row r="904" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="904" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B904" s="29">
         <v>48</v>
       </c>
@@ -26110,7 +25651,7 @@
       </c>
       <c r="K904"/>
     </row>
-    <row r="905" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="905" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B905" s="29">
         <v>43</v>
       </c>
@@ -26122,7 +25663,7 @@
       </c>
       <c r="K905"/>
     </row>
-    <row r="906" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="906" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B906" s="29">
         <v>42</v>
       </c>
@@ -26134,7 +25675,7 @@
       </c>
       <c r="K906"/>
     </row>
-    <row r="907" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="907" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B907" s="29">
         <v>40</v>
       </c>
@@ -26146,7 +25687,7 @@
       </c>
       <c r="K907"/>
     </row>
-    <row r="908" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="908" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B908" s="29">
         <v>37</v>
       </c>
@@ -26158,7 +25699,7 @@
       </c>
       <c r="K908"/>
     </row>
-    <row r="909" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="909" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B909" s="29">
         <v>36</v>
       </c>
@@ -26170,7 +25711,7 @@
       </c>
       <c r="K909"/>
     </row>
-    <row r="910" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="910" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B910" s="29">
         <v>33</v>
       </c>
@@ -26182,7 +25723,7 @@
       </c>
       <c r="K910"/>
     </row>
-    <row r="911" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="911" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B911" s="29">
         <v>32</v>
       </c>
@@ -26194,7 +25735,7 @@
       </c>
       <c r="K911"/>
     </row>
-    <row r="912" spans="2:11" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="912" spans="2:11" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B912" s="29">
         <v>27</v>
       </c>
@@ -26206,7 +25747,7 @@
       </c>
       <c r="K912"/>
     </row>
-    <row r="913" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="913" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B913" s="29">
         <v>23</v>
       </c>
@@ -26218,7 +25759,7 @@
       </c>
       <c r="K913"/>
     </row>
-    <row r="914" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="914" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B914" s="29">
         <v>20</v>
       </c>
@@ -26230,7 +25771,7 @@
       </c>
       <c r="K914"/>
     </row>
-    <row r="915" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="915" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B915" s="29">
         <v>8</v>
       </c>
@@ -26242,14 +25783,14 @@
       </c>
       <c r="K915"/>
     </row>
-    <row r="916" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="916" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="C916" s="7">
         <f>SUM(C855:C915)</f>
         <v>565</v>
       </c>
       <c r="K916"/>
     </row>
-    <row r="917" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="917" spans="1:14" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A917" s="23" t="s">
         <v>380</v>
       </c>
@@ -26263,7 +25804,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="918" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="918" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A918" s="26" t="s">
         <v>42</v>
       </c>
@@ -26294,7 +25835,7 @@
       </c>
       <c r="N918" s="6"/>
     </row>
-    <row r="919" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="919" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B919" s="31" t="s">
         <v>205</v>
       </c>
@@ -26314,7 +25855,7 @@
         <v>0.74629999999999996</v>
       </c>
     </row>
-    <row r="920" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="920" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B920" s="31" t="s">
         <v>206</v>
       </c>
@@ -26334,7 +25875,7 @@
         <v>0.19900000000000001</v>
       </c>
     </row>
-    <row r="921" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="921" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B921" s="31" t="s">
         <v>382</v>
       </c>
@@ -26354,7 +25895,7 @@
         <v>5.4699999999999999E-2</v>
       </c>
     </row>
-    <row r="922" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="922" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="C922" s="7">
         <f>SUM(C919:C921)</f>
         <v>565</v>
@@ -26365,7 +25906,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="923" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="923" spans="1:14" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A923" s="23" t="s">
         <v>383</v>
       </c>
@@ -36234,7 +35775,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="1534" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="1534" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A1534" s="26" t="s">
         <v>42</v>
       </c>
@@ -36269,7 +35810,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="1535" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1535" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1535" s="31" t="s">
         <v>985</v>
       </c>
@@ -36298,7 +35839,7 @@
         <v>0.54730000000000001</v>
       </c>
     </row>
-    <row r="1536" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1536" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1536" s="31" t="s">
         <v>987</v>
       </c>
@@ -36327,7 +35868,7 @@
         <v>0.37309999999999999</v>
       </c>
     </row>
-    <row r="1537" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1537" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1537" s="31" t="s">
         <v>986</v>
       </c>
@@ -36356,7 +35897,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="1538" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1538" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1538" s="31" t="s">
         <v>988</v>
       </c>
@@ -36385,7 +35926,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="1539" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1539" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1539" s="31" t="s">
         <v>989</v>
       </c>
@@ -36414,7 +35955,7 @@
         <v>0.25869999999999999</v>
       </c>
     </row>
-    <row r="1540" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1540" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1540" s="31" t="s">
         <v>990</v>
       </c>
@@ -36443,7 +35984,7 @@
         <v>0.21390000000000001</v>
       </c>
     </row>
-    <row r="1541" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1541" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1541" s="31" t="s">
         <v>991</v>
       </c>
@@ -36472,7 +36013,7 @@
         <v>0.1741</v>
       </c>
     </row>
-    <row r="1542" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1542" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1542" s="31" t="s">
         <v>992</v>
       </c>
@@ -36501,7 +36042,7 @@
         <v>0.15920000000000001</v>
       </c>
     </row>
-    <row r="1543" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1543" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1543" s="31" t="s">
         <v>24</v>
       </c>
@@ -36530,7 +36071,7 @@
         <v>0.1244</v>
       </c>
     </row>
-    <row r="1544" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1544" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B1544" s="31" t="s">
         <v>993</v>
       </c>
@@ -36559,7 +36100,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="1545" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="1545" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="C1545" s="7">
         <f>SUM(C1535:C1544)</f>
         <v>1438</v>
@@ -36569,7 +36110,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="1546" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1546" spans="1:14" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A1546" s="23" t="s">
         <v>994</v>
       </c>
@@ -38316,7 +37857,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="1625" spans="1:14" ht="14" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="1625" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A1625" s="26" t="s">
         <v>1041</v>
       </c>
@@ -38351,7 +37892,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="1626" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1626" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1626" s="9" t="s">
         <v>1060</v>
       </c>
@@ -38380,7 +37921,7 @@
         <v>0.50819999999999999</v>
       </c>
     </row>
-    <row r="1627" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1627" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1627" s="9" t="s">
         <v>1062</v>
       </c>
@@ -38409,7 +37950,7 @@
         <v>0.4536</v>
       </c>
     </row>
-    <row r="1628" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1628" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1628" s="9" t="s">
         <v>1061</v>
       </c>
@@ -38438,7 +37979,7 @@
         <v>0.44259999999999999</v>
       </c>
     </row>
-    <row r="1629" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1629" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1629" s="9" t="s">
         <v>1063</v>
       </c>
@@ -38467,7 +38008,7 @@
         <v>0.377</v>
       </c>
     </row>
-    <row r="1630" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1630" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1630" s="9" t="s">
         <v>1065</v>
       </c>
@@ -38496,7 +38037,7 @@
         <v>0.25679999999999997</v>
       </c>
     </row>
-    <row r="1631" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1631" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1631" s="9" t="s">
         <v>1064</v>
       </c>
@@ -38525,7 +38066,7 @@
         <v>0.25679999999999997</v>
       </c>
     </row>
-    <row r="1632" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1632" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1632" s="9" t="s">
         <v>1066</v>
       </c>
@@ -38554,7 +38095,7 @@
         <v>0.1038</v>
       </c>
     </row>
-    <row r="1633" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1633" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1633" s="9" t="s">
         <v>24</v>
       </c>
@@ -38583,7 +38124,7 @@
         <v>0.1038</v>
       </c>
     </row>
-    <row r="1634" spans="1:14" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="1634" spans="1:14" ht="14" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B1634"/>
       <c r="C1634" s="7">
         <f>SUM(C1626:C1633)</f>
@@ -38594,7 +38135,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="1635" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1635" spans="1:14" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A1635" s="23" t="s">
         <v>1067</v>
       </c>
@@ -41838,9 +41379,6 @@
         <v>38</v>
       </c>
       <c r="D1831" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1831" s="6" t="s">
         <v>1485</v>
       </c>
       <c r="F1831" s="6"/>
@@ -41856,9 +41394,6 @@
         <v>39</v>
       </c>
       <c r="M1831" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1831" s="6" t="s">
         <v>1485</v>
       </c>
     </row>
@@ -41870,9 +41405,6 @@
         <v>283</v>
       </c>
       <c r="D1832" s="1">
-        <v>0.46854304635761601</v>
-      </c>
-      <c r="E1832" s="1">
         <v>0.50088495575221204</v>
       </c>
       <c r="F1832" s="1"/>
@@ -41885,9 +41417,6 @@
         <v>108</v>
       </c>
       <c r="M1832" s="1">
-        <v>0.50939999999999996</v>
-      </c>
-      <c r="N1832" s="1">
         <v>0.5373</v>
       </c>
     </row>
@@ -41899,9 +41428,6 @@
         <v>121</v>
       </c>
       <c r="D1833" s="1">
-        <v>0.20033112582781501</v>
-      </c>
-      <c r="E1833" s="1">
         <v>0.21415929203539799</v>
       </c>
       <c r="F1833" s="1"/>
@@ -41914,9 +41440,6 @@
         <v>38</v>
       </c>
       <c r="M1833" s="1">
-        <v>0.1792</v>
-      </c>
-      <c r="N1833" s="1">
         <v>0.18909999999999999</v>
       </c>
     </row>
@@ -41928,9 +41451,6 @@
         <v>94</v>
       </c>
       <c r="D1834" s="1">
-        <v>0.15562913907284801</v>
-      </c>
-      <c r="E1834" s="1">
         <v>0.16637168141592901</v>
       </c>
       <c r="F1834" s="1"/>
@@ -41943,9 +41463,6 @@
         <v>38</v>
       </c>
       <c r="M1834" s="1">
-        <v>0.1792</v>
-      </c>
-      <c r="N1834" s="1">
         <v>0.18909999999999999</v>
       </c>
     </row>
@@ -41957,9 +41474,6 @@
         <v>90</v>
       </c>
       <c r="D1835" s="1">
-        <v>0.149006622516556</v>
-      </c>
-      <c r="E1835" s="1">
         <v>0.15929203539823</v>
       </c>
       <c r="F1835" s="1"/>
@@ -41972,9 +41486,6 @@
         <v>24</v>
       </c>
       <c r="M1835" s="1">
-        <v>0.1132</v>
-      </c>
-      <c r="N1835" s="1">
         <v>0.11940000000000001</v>
       </c>
     </row>
@@ -41986,9 +41497,6 @@
         <v>8</v>
       </c>
       <c r="D1836" s="1">
-        <v>1.3245033112582801E-2</v>
-      </c>
-      <c r="E1836" s="1">
         <v>1.41592920353982E-2</v>
       </c>
       <c r="F1836" s="1"/>
@@ -42001,9 +41509,6 @@
         <v>2</v>
       </c>
       <c r="M1836" s="1">
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="N1836" s="1">
         <v>0.01</v>
       </c>
     </row>
@@ -42015,9 +41520,6 @@
         <v>8</v>
       </c>
       <c r="D1837" s="1">
-        <v>1.3245033112582801E-2</v>
-      </c>
-      <c r="E1837" s="1">
         <v>1.41592920353982E-2</v>
       </c>
       <c r="F1837" s="1"/>
@@ -42030,9 +41532,6 @@
         <v>2</v>
       </c>
       <c r="M1837" s="1">
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="N1837" s="1">
         <v>0.01</v>
       </c>
     </row>
@@ -49888,18 +49387,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D488:D492">
-    <cfRule type="colorScale" priority="349">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C488:C492">
     <cfRule type="dataBar" priority="348">
       <dataBar>
@@ -49912,18 +49399,6 @@
           <x14:id>{369FFAC0-2DD5-4E0B-92AA-7D123B7EF4FC}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M488:M492">
-    <cfRule type="colorScale" priority="347">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L488:L492">
@@ -50044,18 +49519,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M548:M565">
-    <cfRule type="colorScale" priority="337">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L548:L565">
     <cfRule type="dataBar" priority="336">
       <dataBar>
@@ -50068,18 +49531,6 @@
           <x14:id>{FA81182E-B05C-4582-B108-54022B0F64EF}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D548:D565">
-    <cfRule type="colorScale" priority="335">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C548:C565">
@@ -50290,7 +49741,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D630:H653">
+  <conditionalFormatting sqref="F630:H653 D630:D653">
     <cfRule type="colorScale" priority="302">
       <colorScale>
         <cfvo type="min"/>
@@ -50314,18 +49765,6 @@
           <x14:id>{0F719FDF-5AE8-45E9-B7C0-538626A32A25}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M630:N652">
-    <cfRule type="colorScale" priority="300">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C657:C736">
@@ -50394,7 +49833,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D740:H750">
+  <conditionalFormatting sqref="F740:H750 D740:D750">
     <cfRule type="colorScale" priority="294">
       <colorScale>
         <cfvo type="min"/>
@@ -50418,18 +49857,6 @@
           <x14:id>{A3B94379-DC6C-4CA3-9ED7-64B320723696}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M740:N750">
-    <cfRule type="colorScale" priority="292">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M754:M762">
@@ -50616,19 +50043,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E488:H492">
-    <cfRule type="colorScale" priority="276">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N488:N492">
+  <conditionalFormatting sqref="M488:M492">
     <cfRule type="colorScale" priority="275">
       <colorScale>
         <cfvo type="min"/>
@@ -50664,19 +50079,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E548:H565">
-    <cfRule type="colorScale" priority="272">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N548:N565">
+  <conditionalFormatting sqref="M548:M565">
     <cfRule type="colorScale" priority="271">
       <colorScale>
         <cfvo type="min"/>
@@ -52064,18 +51467,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1832:N1837">
-    <cfRule type="colorScale" priority="149">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L1832:L1837">
     <cfRule type="dataBar" priority="148">
       <dataBar>
@@ -52090,7 +51481,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1832:H1837">
+  <conditionalFormatting sqref="F1832:H1837 D1832:D1837">
     <cfRule type="colorScale" priority="147">
       <colorScale>
         <cfvo type="min"/>
@@ -53980,6 +53371,66 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="F784:F788">
     <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1832:M1837">
+    <cfRule type="colorScale" priority="535">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F488:H492 D488:D492">
+    <cfRule type="colorScale" priority="536">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F548:H565 D548:D565">
+    <cfRule type="colorScale" priority="537">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M740:M750">
+    <cfRule type="colorScale" priority="538">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M630:M652">
+    <cfRule type="colorScale" priority="539">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>